<commit_message>
Notes and tasks clean up.
</commit_message>
<xml_diff>
--- a/Support/ThemeTasks.xlsx
+++ b/Support/ThemeTasks.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesMc\Data\Clients\DigitalZenWorks\DigitalZenTheme\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB5DCBA-134D-4D65-83E2-83B0F523049B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="Finished" sheetId="2" r:id="rId2"/>
-    <sheet name="Frozen" sheetId="4" r:id="rId3"/>
-    <sheet name="CheckList" sheetId="3" r:id="rId4"/>
+    <sheet name="Revised" sheetId="5" r:id="rId2"/>
+    <sheet name="Finished" sheetId="2" r:id="rId3"/>
+    <sheet name="Frozen" sheetId="4" r:id="rId4"/>
+    <sheet name="CheckList" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="286">
   <si>
     <t>Priority</t>
   </si>
@@ -827,12 +829,75 @@
   </si>
   <si>
     <t>Changed directory structure to CommandLineTools</t>
+  </si>
+  <si>
+    <t>Added npm package.json file for build support.</t>
+  </si>
+  <si>
+    <t>Added ignore file.</t>
+  </si>
+  <si>
+    <t>Added grunt build task runner.</t>
+  </si>
+  <si>
+    <t>Added grunt file.</t>
+  </si>
+  <si>
+    <t>Added build command.</t>
+  </si>
+  <si>
+    <t>Other grunt things</t>
+  </si>
+  <si>
+    <t>Added repository info, moved author and license to top, added grunt-contrib-cssmin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Added components from boilerplate template.</t>
+  </si>
+  <si>
+    <t>Added support to detect production/development environments and set the type of css file based on that.</t>
+  </si>
+  <si>
+    <t>Added sass, uglify and watch packages.</t>
+  </si>
+  <si>
+    <t>Integrated HTML from _s starter theme.</t>
+  </si>
+  <si>
+    <t>Added standard license.</t>
+  </si>
+  <si>
+    <t>Added blank screen shot.</t>
+  </si>
+  <si>
+    <t>Added developer support notes.</t>
+  </si>
+  <si>
+    <t>Added code sniffer control file.</t>
+  </si>
+  <si>
+    <t>Added sniff support, composer checking and zipping to build process.</t>
+  </si>
+  <si>
+    <t>Ignore generated zip file.</t>
+  </si>
+  <si>
+    <t>Default .editorconfig file.</t>
+  </si>
+  <si>
+    <t>Added Visual Studio Code workspace.</t>
+  </si>
+  <si>
+    <t>Initial commit</t>
+  </si>
+  <si>
+    <t>Composer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1194,12 +1259,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1330,56 +1395,6 @@
         <v>43990</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="10">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="10">
-        <v>14</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M7" s="11"/>
-    </row>
     <row r="8" spans="1:15">
       <c r="A8" s="14" t="s">
         <v>200</v>
@@ -1433,57 +1448,6 @@
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B10">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>218</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>218</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>218</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="1">
-        <v>43712</v>
-      </c>
-    </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>200</v>
@@ -1501,26 +1465,6 @@
         <v>43712</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B14">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>218</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="1">
-        <v>43712</v>
-      </c>
-      <c r="M14" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>200</v>
@@ -1535,26 +1479,6 @@
         <v>209</v>
       </c>
       <c r="L15" s="1">
-        <v>43976</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16">
-        <v>108</v>
-      </c>
-      <c r="D16" t="s">
-        <v>218</v>
-      </c>
-      <c r="E16" t="s">
-        <v>227</v>
-      </c>
-      <c r="G16" t="s">
-        <v>217</v>
-      </c>
-      <c r="L16" s="1">
         <v>43976</v>
       </c>
     </row>
@@ -4522,7 +4446,7 @@
       <c r="O193" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:R193">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R193">
     <sortCondition ref="A2:A193"/>
     <sortCondition ref="B2:B193"/>
   </sortState>
@@ -4532,11 +4456,266 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A9387A-1D57-4945-8BD2-D7382FB60507}">
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:L61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="G2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="G3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="G4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="G5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="G6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="G8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="10">
+        <v>12</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="15">
+        <v>43986</v>
+      </c>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="10">
+        <v>14</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="15">
+        <v>43986</v>
+      </c>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>218</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>218</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>218</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="1">
+        <v>43712</v>
+      </c>
+      <c r="M14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L15" s="1">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7">
+      <c r="G18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7">
+      <c r="G21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7">
+      <c r="G22" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7">
+      <c r="G23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5337,13 +5516,63 @@
         <v>43986</v>
       </c>
     </row>
+    <row r="62" spans="1:13">
+      <c r="G62" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="G63" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="G64" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7">
+      <c r="G65" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7">
+      <c r="G66" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7">
+      <c r="G67" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7">
+      <c r="G68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7">
+      <c r="G69" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7">
+      <c r="G70" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7">
+      <c r="G71" t="s">
+        <v>269</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5380,8 +5609,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Notes and tasks updates.
</commit_message>
<xml_diff>
--- a/Support/ThemeTasks.xlsx
+++ b/Support/ThemeTasks.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesMc\Data\Clients\DigitalZenWorks\DigitalZenTheme\Support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesMc\Data\Clients\DigitalZenWorks\DigitalZenThemePrevious\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB5DCBA-134D-4D65-83E2-83B0F523049B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26738B9-CDBA-43B6-B466-1E8D4E86328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="Revised" sheetId="5" r:id="rId2"/>
-    <sheet name="Finished" sheetId="2" r:id="rId3"/>
-    <sheet name="Frozen" sheetId="4" r:id="rId4"/>
-    <sheet name="CheckList" sheetId="3" r:id="rId5"/>
+    <sheet name="Finished" sheetId="2" r:id="rId2"/>
+    <sheet name="Frozen" sheetId="4" r:id="rId3"/>
+    <sheet name="CheckList" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="335">
   <si>
     <t>Priority</t>
   </si>
@@ -892,6 +891,153 @@
   </si>
   <si>
     <t>Composer</t>
+  </si>
+  <si>
+    <t>Create GitHub repo</t>
+  </si>
+  <si>
+    <t>gitignore vendor &amp; node_modules</t>
+  </si>
+  <si>
+    <t>git add package-lock.json package.json</t>
+  </si>
+  <si>
+    <t>Create index.php</t>
+  </si>
+  <si>
+    <t>Edit index.php comments</t>
+  </si>
+  <si>
+    <t>npm install grunt-contrib-cssmin --save-dev</t>
+  </si>
+  <si>
+    <t>Edit Gruntfile.js to include cssmin</t>
+  </si>
+  <si>
+    <t>create build.cmd</t>
+  </si>
+  <si>
+    <t>Add grunt cssmin to build</t>
+  </si>
+  <si>
+    <t>build.cmd</t>
+  </si>
+  <si>
+    <t>Create header.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link rel="stylesheet" href="&lt;?php echo $theme_directory; ?&gt;/css/normalize.css"&gt;</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
+    <t>Added components from boilerplate template.</t>
+  </si>
+  <si>
+    <t>figure out why show_main_menu is always false</t>
+  </si>
+  <si>
+    <t>Review mujin.ai about menu support</t>
+  </si>
+  <si>
+    <t>Find a way to export / import plugin settings</t>
+  </si>
+  <si>
+    <t>Find a way to export / import customization settings</t>
+  </si>
+  <si>
+    <t>The "dealerdirect/phpcodesniffer-composer-installer" plugin was skipped because it requires a Plugin API version ("^1.0") that does not match your Composer installation ("2.0.0"). You may need to run composer update with the "--no-plugins" option.</t>
+  </si>
+  <si>
+    <t>Error: No files matching the pattern "'assets/css/*.css'" were found.</t>
+  </si>
+  <si>
+    <t>at DigitalZenTheme\SourceCode\node_modules\stylelint\lib\standalone.js:212:12</t>
+  </si>
+  <si>
+    <t>at processTicksAndRejections (internal/process/task_queues.js:93:5)</t>
+  </si>
+  <si>
+    <t>Error: No files matching the pattern "'*.css'" were found.</t>
+  </si>
+  <si>
+    <t>Deprecation Warning: 'declaration-property-unit-whitelist' has been deprecated. Instead use 'declaration-property-unit-allowed-list'. See: https://github.com/stylelint/stylelint/blob/13.7.0/lib/rules/declaration-property-unit-whitelist/README.md</t>
+  </si>
+  <si>
+    <t>The "digital-zen" prefix is not a valid</t>
+  </si>
+  <si>
+    <t>namespace/function/class/variable/constant prefix in PHP.</t>
+  </si>
+  <si>
+    <t>WordPress.NamingConventions.PrefixAllGlobals.InvalidPrefixPassed</t>
+  </si>
+  <si>
+    <t>The prefix is not a valid namespace/function/class/variable/constant prefix in PHP.</t>
+  </si>
+  <si>
+    <t>Global variables defined by a theme/plugin should start with the theme/plugin prefix. Found:</t>
+  </si>
+  <si>
+    <t>$digitalzen_archive_content.</t>
+  </si>
+  <si>
+    <t>WordPress.NamingConventions.PrefixAllGlobals.NonPrefixedVariableFound</t>
+  </si>
+  <si>
+    <t>Global variables defined by a theme/plugin should start with the theme/plugin prefix. dash</t>
+  </si>
+  <si>
+    <t>Edit theme for menu support</t>
+  </si>
+  <si>
+    <t>Added customization from admin</t>
+  </si>
+  <si>
+    <t>**Manual step</t>
+  </si>
+  <si>
+    <t>Edit theme for menu override support</t>
+  </si>
+  <si>
+    <t>language_attributes() vs my language functions</t>
+  </si>
+  <si>
+    <t>bloginfo( 'charset' ); vs utf-8</t>
+  </si>
+  <si>
+    <t>Merge ALL css into one file</t>
+  </si>
+  <si>
+    <t>( ! ) Notice: Undefined variable: component in C:\Util\xampp\htdocs\wp\wp-content\themes\DigitalZen\header.php on line 41</t>
+  </si>
+  <si>
+    <t>Added unchecked readme.txt from _s generation.</t>
+  </si>
+  <si>
+    <t>Moved js files to assets.</t>
+  </si>
+  <si>
+    <t>Added common.scss.</t>
+  </si>
+  <si>
+    <t>Added js/vendor files.</t>
+  </si>
+  <si>
+    <t>Added initial language support.</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Make New Theme Repo</t>
   </si>
 </sst>
 </file>
@@ -951,7 +1097,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -980,6 +1126,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,9 +1410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1320,237 +1468,305 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="11" t="s">
+      <c r="G2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="11">
-        <v>2</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M2" s="11"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
+      <c r="B3" s="10">
+        <v>12</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" t="s">
         <v>218</v>
       </c>
-      <c r="G3" t="s">
-        <v>260</v>
-      </c>
-      <c r="L3" s="1">
-        <v>43994</v>
-      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="15">
+        <v>43986</v>
+      </c>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
+      <c r="B4" s="10">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11"/>
       <c r="D4" t="s">
         <v>218</v>
       </c>
-      <c r="G4" t="s">
-        <v>252</v>
-      </c>
-      <c r="L4" s="1">
-        <v>43990</v>
-      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="15">
+        <v>43986</v>
+      </c>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>200</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>218</v>
       </c>
       <c r="G5" t="s">
-        <v>253</v>
+        <v>33</v>
       </c>
       <c r="L5" s="1">
-        <v>43990</v>
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="1">
+        <v>43712</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="14" t="s">
+      <c r="A8" t="s">
         <v>200</v>
       </c>
-      <c r="B8" s="10">
-        <v>15</v>
-      </c>
-      <c r="C8" s="10"/>
+      <c r="B8">
+        <v>42</v>
+      </c>
       <c r="D8" t="s">
         <v>218</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M8" s="13"/>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1">
+        <v>43712</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="11" t="s">
+      <c r="A9" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="11">
-        <v>20</v>
-      </c>
-      <c r="C9" s="11"/>
+      <c r="B9">
+        <v>108</v>
+      </c>
       <c r="D9" t="s">
         <v>218</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>218</v>
-      </c>
+      <c r="E9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" t="s">
+        <v>217</v>
+      </c>
+      <c r="L9" s="1">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="G10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="G11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="18" customFormat="1">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:15" s="18" customFormat="1">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
       <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="1">
-        <v>43712</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:15" s="18" customFormat="1">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>200</v>
       </c>
       <c r="B15">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>218</v>
       </c>
       <c r="G15" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="L15" s="1">
-        <v>43976</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" t="s">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="B17">
-        <v>109</v>
-      </c>
+      <c r="B16" s="10">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="15">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="11">
+        <v>20</v>
+      </c>
+      <c r="C17" s="11"/>
       <c r="D17" t="s">
         <v>218</v>
       </c>
-      <c r="E17" t="s">
-        <v>227</v>
-      </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="15">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>200</v>
       </c>
       <c r="B18">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
         <v>218</v>
       </c>
-      <c r="E18" t="s">
-        <v>227</v>
-      </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1">
-        <v>43661</v>
-      </c>
-      <c r="M18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>200</v>
       </c>
       <c r="B19">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
         <v>218</v>
       </c>
-      <c r="E19" t="s">
-        <v>227</v>
-      </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="L19" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>200</v>
       </c>
       <c r="B20">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
         <v>218</v>
@@ -1559,18 +1775,18 @@
         <v>227</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="L20" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>200</v>
       </c>
       <c r="B21">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
         <v>218</v>
@@ -1579,18 +1795,21 @@
         <v>227</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="L21" s="1">
         <v>43661</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="M21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>200</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
         <v>218</v>
@@ -1599,18 +1818,18 @@
         <v>227</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="L22" s="1">
         <v>43661</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>200</v>
       </c>
       <c r="B23">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
         <v>218</v>
@@ -1619,254 +1838,260 @@
         <v>227</v>
       </c>
       <c r="G23" t="s">
-        <v>229</v>
+        <v>61</v>
       </c>
       <c r="L23" s="1">
         <v>43661</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>200</v>
       </c>
       <c r="B24">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
         <v>218</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L24" s="1">
-        <v>43660</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+        <v>43661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>200</v>
       </c>
       <c r="B25">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>218</v>
       </c>
       <c r="E25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L25" s="1">
-        <v>43660</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>43661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>200</v>
       </c>
       <c r="B26">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D26" t="s">
         <v>218</v>
       </c>
       <c r="E26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>229</v>
       </c>
       <c r="L26" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+        <v>43661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>200</v>
       </c>
       <c r="B27">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
         <v>218</v>
       </c>
+      <c r="E27" t="s">
+        <v>228</v>
+      </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="L27" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+        <v>43660</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>200</v>
       </c>
       <c r="B28">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
         <v>218</v>
       </c>
+      <c r="E28" t="s">
+        <v>228</v>
+      </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="L28" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+        <v>43660</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>200</v>
       </c>
       <c r="B29">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D29" t="s">
         <v>218</v>
       </c>
+      <c r="E29" t="s">
+        <v>228</v>
+      </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="L29" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>200</v>
       </c>
       <c r="B30">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
         <v>218</v>
       </c>
       <c r="G30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L30" s="1">
         <v>43661</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>200</v>
       </c>
       <c r="B31">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
         <v>218</v>
       </c>
-      <c r="E31" t="s">
-        <v>228</v>
-      </c>
       <c r="G31" t="s">
-        <v>229</v>
+        <v>72</v>
       </c>
       <c r="L31" s="1">
         <v>43661</v>
       </c>
-      <c r="O31" s="7"/>
-    </row>
-    <row r="32" spans="1:15" ht="15.75">
-      <c r="A32" s="6" t="s">
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
         <v>200</v>
       </c>
-      <c r="B32" s="7">
-        <v>150</v>
-      </c>
-      <c r="C32" s="7"/>
+      <c r="B32">
+        <v>140</v>
+      </c>
       <c r="D32" t="s">
         <v>218</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="G32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="2">
-        <v>42636</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="1">
+        <v>43661</v>
+      </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>200</v>
       </c>
       <c r="B33">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
         <v>218</v>
       </c>
       <c r="G33" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="L33" s="1">
-        <v>43712</v>
+        <v>43661</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="E34" t="s">
+        <v>228</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
       <c r="L34" s="1">
-        <v>43660</v>
-      </c>
-      <c r="M34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35">
-        <v>33</v>
-      </c>
+        <v>43661</v>
+      </c>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.75">
+      <c r="A35" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" s="7">
+        <v>150</v>
+      </c>
+      <c r="C35" s="7"/>
       <c r="D35" t="s">
-        <v>220</v>
-      </c>
-      <c r="G35" t="s">
-        <v>13</v>
-      </c>
-      <c r="L35" s="1">
-        <v>43712</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="2">
+        <v>42636</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="L36" s="1">
         <v>43712</v>
@@ -1877,16 +2102,19 @@
         <v>95</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
         <v>220</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L37" s="1">
-        <v>43712</v>
+        <v>43660</v>
+      </c>
+      <c r="M37" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -1894,13 +2122,13 @@
         <v>95</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
         <v>220</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L38" s="1">
         <v>43712</v>
@@ -1911,13 +2139,13 @@
         <v>95</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
         <v>220</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L39" s="1">
         <v>43712</v>
@@ -1928,13 +2156,13 @@
         <v>95</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D40" t="s">
         <v>220</v>
       </c>
       <c r="G40" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L40" s="1">
         <v>43712</v>
@@ -1945,13 +2173,13 @@
         <v>95</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D41" t="s">
         <v>220</v>
       </c>
       <c r="G41" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="L41" s="1">
         <v>43712</v>
@@ -1962,13 +2190,13 @@
         <v>95</v>
       </c>
       <c r="B42">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s">
         <v>220</v>
       </c>
       <c r="G42" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="L42" s="1">
         <v>43712</v>
@@ -1979,13 +2207,13 @@
         <v>95</v>
       </c>
       <c r="B43">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
         <v>220</v>
       </c>
       <c r="G43" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L43" s="1">
         <v>43712</v>
@@ -1996,134 +2224,107 @@
         <v>95</v>
       </c>
       <c r="B44">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
         <v>220</v>
       </c>
       <c r="G44" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="L44" s="1">
-        <v>43665</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="15.75">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>95</v>
       </c>
       <c r="B45">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
         <v>220</v>
       </c>
       <c r="G45" t="s">
-        <v>68</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="L45" s="2">
-        <v>42636</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="15.75">
-      <c r="A46" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="L45" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
       <c r="D46" t="s">
         <v>220</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="G46" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J46" s="7"/>
-      <c r="L46" s="2">
-        <v>42636</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-    </row>
-    <row r="47" spans="1:15" ht="15.75">
-      <c r="A47" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+      <c r="G46" t="s">
+        <v>39</v>
+      </c>
+      <c r="L46" s="1">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
       <c r="D47" t="s">
         <v>220</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J47" s="7"/>
-      <c r="L47" s="2">
-        <v>42636</v>
-      </c>
-      <c r="M47" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="A48" s="3" t="s">
+      <c r="G47" t="s">
+        <v>67</v>
+      </c>
+      <c r="L47" s="1">
+        <v>43665</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75">
+      <c r="A48" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="B48">
+        <v>48</v>
+      </c>
       <c r="D48" t="s">
         <v>220</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="G48" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="8">
-        <v>42754</v>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L48" s="2">
+        <v>42636</v>
       </c>
       <c r="M48" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
     </row>
     <row r="49" spans="1:18" ht="15.75">
       <c r="A49" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" t="s">
         <v>220</v>
       </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="E49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="J49" s="7"/>
       <c r="L49" s="2">
@@ -2135,205 +2336,220 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
     </row>
-    <row r="50" spans="1:18">
-      <c r="A50" t="s">
-        <v>95</v>
-      </c>
+    <row r="50" spans="1:18" ht="15.75">
+      <c r="A50" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
       <c r="D50" t="s">
         <v>220</v>
       </c>
-      <c r="G50" t="s">
-        <v>141</v>
-      </c>
-      <c r="L50" s="1">
-        <v>43712</v>
+      <c r="E50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J50" s="7"/>
+      <c r="L50" s="2">
+        <v>42636</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" ht="15.75">
-      <c r="A51" s="5" t="s">
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
       <c r="D51" t="s">
         <v>220</v>
       </c>
-      <c r="G51" t="s">
-        <v>152</v>
-      </c>
-      <c r="L51" s="1">
-        <v>43712</v>
+      <c r="E51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="8">
+        <v>42754</v>
       </c>
       <c r="M51" s="7" t="s">
         <v>198</v>
       </c>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
     </row>
     <row r="52" spans="1:18" ht="15.75">
       <c r="A52" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="7" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" t="s">
+        <v>220</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J52" s="7"/>
+      <c r="L52" s="2">
+        <v>42636</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>220</v>
+      </c>
+      <c r="G53" t="s">
+        <v>141</v>
+      </c>
+      <c r="L53" s="1">
+        <v>43712</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="15.75">
+      <c r="A54" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" t="s">
+        <v>220</v>
+      </c>
+      <c r="G54" t="s">
+        <v>152</v>
+      </c>
+      <c r="L54" s="1">
+        <v>43712</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="15.75">
+      <c r="A55" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="3" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H52" s="7"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="8">
+      <c r="H55" s="7"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="8">
         <v>42754</v>
       </c>
-      <c r="M52" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="O52" s="4"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-    </row>
-    <row r="53" spans="1:18">
-      <c r="A53" s="7" t="s">
+      <c r="M55" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="O55" s="4"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7" t="s">
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="8">
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="8">
         <v>42556</v>
       </c>
-      <c r="M53" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="15.75">
-      <c r="A54" s="6" t="s">
+      <c r="M56" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="15.75">
+      <c r="A57" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="7" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="3" t="s">
+      <c r="E57" s="3"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="8">
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="8">
         <v>42754</v>
       </c>
-      <c r="M54" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18">
-      <c r="A55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>219</v>
-      </c>
-      <c r="G55" t="s">
-        <v>204</v>
-      </c>
-      <c r="H55" t="s">
-        <v>205</v>
-      </c>
-      <c r="L55" s="1">
-        <v>43660</v>
-      </c>
-      <c r="M55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="15.75">
-      <c r="A56" t="s">
-        <v>120</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" t="s">
-        <v>66</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="L56" s="1">
-        <v>43719</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="15.75">
-      <c r="A57" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57">
-        <v>8</v>
-      </c>
-      <c r="D57" t="s">
-        <v>219</v>
-      </c>
-      <c r="F57" s="4"/>
-      <c r="G57" t="s">
-        <v>66</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="L57" s="1">
-        <v>43719</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="15.75">
+      <c r="M57" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" t="s">
         <v>120</v>
       </c>
       <c r="B58">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D58" t="s">
         <v>219</v>
       </c>
-      <c r="F58" s="4"/>
       <c r="G58" t="s">
-        <v>66</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>213</v>
+        <v>204</v>
+      </c>
+      <c r="H58" t="s">
+        <v>205</v>
       </c>
       <c r="L58" s="1">
-        <v>43719</v>
+        <v>43660</v>
+      </c>
+      <c r="M58" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -4325,11 +4541,78 @@
         <v>198</v>
       </c>
     </row>
+    <row r="152" spans="1:13">
+      <c r="G152" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
+      <c r="G153" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
+      <c r="G154" t="s">
+        <v>304</v>
+      </c>
+    </row>
     <row r="155" spans="1:13">
+      <c r="G155" t="s">
+        <v>305</v>
+      </c>
       <c r="M155" s="11"/>
     </row>
+    <row r="156" spans="1:13">
+      <c r="G156" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
+      <c r="G157" t="s">
+        <v>307</v>
+      </c>
+      <c r="H157" t="s">
+        <v>308</v>
+      </c>
+      <c r="I157" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
+      <c r="G158" t="s">
+        <v>310</v>
+      </c>
+      <c r="H158" t="s">
+        <v>308</v>
+      </c>
+      <c r="I158" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
+      <c r="G159" t="s">
+        <v>311</v>
+      </c>
+    </row>
     <row r="160" spans="1:13">
+      <c r="G160" t="s">
+        <v>312</v>
+      </c>
+      <c r="H160" t="s">
+        <v>313</v>
+      </c>
+      <c r="I160" t="s">
+        <v>314</v>
+      </c>
       <c r="L160" s="1"/>
+    </row>
+    <row r="161" spans="1:13">
+      <c r="G161" t="s">
+        <v>315</v>
+      </c>
+      <c r="H161" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="162" spans="1:13">
       <c r="A162" s="11"/>
@@ -4338,9 +4621,15 @@
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
       <c r="F162" s="11"/>
-      <c r="G162" s="11"/>
-      <c r="H162" s="11"/>
-      <c r="I162" s="11"/>
+      <c r="G162" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="H162" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="I162" s="11" t="s">
+        <v>318</v>
+      </c>
       <c r="J162" s="11"/>
       <c r="K162" s="11"/>
       <c r="L162" s="15"/>
@@ -4353,7 +4642,9 @@
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
       <c r="F163" s="11"/>
-      <c r="G163" s="11"/>
+      <c r="G163" s="11" t="s">
+        <v>319</v>
+      </c>
       <c r="H163" s="11"/>
       <c r="I163" s="11"/>
       <c r="J163" s="11"/>
@@ -4368,6 +4659,9 @@
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
       <c r="F164" s="11"/>
+      <c r="G164" t="s">
+        <v>320</v>
+      </c>
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
       <c r="J164" s="11"/>
@@ -4376,68 +4670,169 @@
       <c r="M164" s="11"/>
     </row>
     <row r="165" spans="1:13">
+      <c r="G165" t="s">
+        <v>321</v>
+      </c>
+      <c r="H165" t="s">
+        <v>322</v>
+      </c>
       <c r="L165" s="1"/>
     </row>
     <row r="166" spans="1:13">
+      <c r="G166" t="s">
+        <v>323</v>
+      </c>
       <c r="L166" s="1"/>
     </row>
     <row r="167" spans="1:13">
+      <c r="G167" t="s">
+        <v>324</v>
+      </c>
       <c r="L167" s="1"/>
     </row>
     <row r="168" spans="1:13">
+      <c r="G168" t="s">
+        <v>325</v>
+      </c>
       <c r="L168" s="1"/>
     </row>
     <row r="169" spans="1:13">
+      <c r="G169" t="s">
+        <v>326</v>
+      </c>
       <c r="L169" s="1"/>
     </row>
     <row r="170" spans="1:13">
+      <c r="G170" t="s">
+        <v>327</v>
+      </c>
       <c r="L170" s="1"/>
     </row>
     <row r="171" spans="1:13">
+      <c r="D171" t="s">
+        <v>333</v>
+      </c>
+      <c r="G171" t="s">
+        <v>276</v>
+      </c>
       <c r="L171" s="1"/>
     </row>
     <row r="172" spans="1:13">
+      <c r="D172" t="s">
+        <v>333</v>
+      </c>
+      <c r="G172" t="s">
+        <v>277</v>
+      </c>
       <c r="L172" s="1"/>
     </row>
     <row r="173" spans="1:13">
+      <c r="D173" t="s">
+        <v>333</v>
+      </c>
+      <c r="G173" t="s">
+        <v>328</v>
+      </c>
       <c r="L173" s="1"/>
     </row>
     <row r="174" spans="1:13">
+      <c r="D174" t="s">
+        <v>333</v>
+      </c>
+      <c r="G174" t="s">
+        <v>282</v>
+      </c>
       <c r="L174" s="1"/>
     </row>
     <row r="175" spans="1:13">
+      <c r="D175" t="s">
+        <v>333</v>
+      </c>
+      <c r="G175" t="s">
+        <v>283</v>
+      </c>
       <c r="L175" s="1"/>
     </row>
     <row r="176" spans="1:13">
+      <c r="D176" t="s">
+        <v>333</v>
+      </c>
+      <c r="G176" t="s">
+        <v>265</v>
+      </c>
       <c r="L176" s="1"/>
     </row>
-    <row r="177" spans="6:12">
+    <row r="177" spans="4:12">
+      <c r="D177" t="s">
+        <v>333</v>
+      </c>
+      <c r="G177" t="s">
+        <v>267</v>
+      </c>
       <c r="L177" s="1"/>
     </row>
-    <row r="178" spans="6:12">
+    <row r="178" spans="4:12">
+      <c r="D178" t="s">
+        <v>333</v>
+      </c>
+      <c r="G178" t="s">
+        <v>268</v>
+      </c>
       <c r="L178" s="1"/>
     </row>
-    <row r="179" spans="6:12">
+    <row r="179" spans="4:12">
+      <c r="D179" t="s">
+        <v>333</v>
+      </c>
+      <c r="G179" t="s">
+        <v>269</v>
+      </c>
       <c r="L179" s="1"/>
     </row>
-    <row r="180" spans="6:12">
+    <row r="180" spans="4:12">
+      <c r="D180" t="s">
+        <v>333</v>
+      </c>
+      <c r="G180" t="s">
+        <v>329</v>
+      </c>
       <c r="L180" s="1"/>
     </row>
-    <row r="181" spans="6:12">
+    <row r="181" spans="4:12">
+      <c r="D181" t="s">
+        <v>333</v>
+      </c>
+      <c r="G181" t="s">
+        <v>330</v>
+      </c>
       <c r="L181" s="1"/>
     </row>
-    <row r="182" spans="6:12">
+    <row r="182" spans="4:12">
+      <c r="D182" t="s">
+        <v>333</v>
+      </c>
+      <c r="G182" t="s">
+        <v>331</v>
+      </c>
       <c r="L182" s="1"/>
     </row>
-    <row r="188" spans="6:12" ht="15.75">
+    <row r="183" spans="4:12">
+      <c r="D183" t="s">
+        <v>333</v>
+      </c>
+      <c r="G183" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="188" spans="4:12" ht="15.75">
       <c r="F188" s="4"/>
       <c r="H188" s="4"/>
     </row>
-    <row r="189" spans="6:12" ht="15.75">
+    <row r="189" spans="4:12" ht="15.75">
       <c r="F189" s="4"/>
       <c r="H189" s="4"/>
     </row>
-    <row r="190" spans="6:12" ht="15.75">
+    <row r="190" spans="4:12" ht="15.75">
       <c r="F190" s="4"/>
       <c r="H190" s="4"/>
     </row>
@@ -4456,266 +4851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A9387A-1D57-4945-8BD2-D7382FB60507}">
-  <dimension ref="A1:M23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="7" width="47" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="15.75">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="G2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="G3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="G4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="G5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="G6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="G8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B9" s="10">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" t="s">
-        <v>218</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B10" s="10">
-        <v>14</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" t="s">
-        <v>218</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="15">
-        <v>43986</v>
-      </c>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>218</v>
-      </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>218</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>200</v>
-      </c>
-      <c r="B13">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>218</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B14">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>218</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="1">
-        <v>43712</v>
-      </c>
-      <c r="M14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15">
-        <v>108</v>
-      </c>
-      <c r="D15" t="s">
-        <v>218</v>
-      </c>
-      <c r="E15" t="s">
-        <v>227</v>
-      </c>
-      <c r="G15" t="s">
-        <v>217</v>
-      </c>
-      <c r="L15" s="1">
-        <v>43976</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7">
-      <c r="G21" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7">
-      <c r="G22" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7">
-      <c r="G23" t="s">
-        <v>278</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M71"/>
-  <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116:G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5531,39 +5671,382 @@
         <v>282</v>
       </c>
     </row>
-    <row r="65" spans="7:7">
+    <row r="65" spans="1:13">
       <c r="G65" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="7:7">
+    <row r="66" spans="1:13">
       <c r="G66" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="7:7">
+    <row r="67" spans="1:13">
       <c r="G67" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="68" spans="7:7">
+    <row r="68" spans="1:13">
       <c r="G68" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="7:7">
+    <row r="69" spans="1:13">
       <c r="G69" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="7:7">
+    <row r="70" spans="1:13">
       <c r="G70" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="7:7">
+    <row r="71" spans="1:13">
       <c r="G71" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" s="11">
+        <v>2</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" t="s">
+        <v>218</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="15">
+        <v>43986</v>
+      </c>
+      <c r="M72" s="11"/>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>218</v>
+      </c>
+      <c r="G73" t="s">
+        <v>260</v>
+      </c>
+      <c r="L73" s="1">
+        <v>43994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B74" s="18">
+        <v>11</v>
+      </c>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="19">
+        <v>43990</v>
+      </c>
+      <c r="M74" s="18"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.75">
+      <c r="A75" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>219</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L75" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="15.75">
+      <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>219</v>
+      </c>
+      <c r="F76" s="4"/>
+      <c r="G76" t="s">
+        <v>66</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="L76" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="15.75">
+      <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>219</v>
+      </c>
+      <c r="F77" s="4"/>
+      <c r="G77" t="s">
+        <v>66</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="L77" s="1">
+        <v>43719</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="G78" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="G79" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="G80" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="7:8">
+      <c r="G81" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="82" spans="7:8">
+      <c r="G82" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="83" spans="7:8">
+      <c r="G83" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="84" spans="7:8">
+      <c r="G84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="7:8">
+      <c r="G85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="7:8">
+      <c r="G86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="7:8">
+      <c r="G87" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="7:8">
+      <c r="G88" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="7:8">
+      <c r="G89" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="7:8">
+      <c r="G90" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="7:8">
+      <c r="G91" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="92" spans="7:8">
+      <c r="G92" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="93" spans="7:8">
+      <c r="G93" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="94" spans="7:8">
+      <c r="G94" t="s">
+        <v>292</v>
+      </c>
+      <c r="H94" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="7:8">
+      <c r="G95" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="96" spans="7:8">
+      <c r="G96" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8">
+      <c r="G97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="7:8">
+      <c r="G98" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="7:8">
+      <c r="G99" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100" spans="7:8">
+      <c r="G100" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="101" spans="7:8">
+      <c r="G101" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="7:8">
+      <c r="G102" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="7:8">
+      <c r="G103" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="7:8">
+      <c r="G104" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="7:8">
+      <c r="G105" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="7:8">
+      <c r="G106" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="107" spans="7:8">
+      <c r="G107" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="108" spans="7:8">
+      <c r="G108" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="109" spans="7:8">
+      <c r="G109" t="s">
+        <v>42</v>
+      </c>
+      <c r="H109" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="110" spans="7:8">
+      <c r="G110" t="s">
+        <v>42</v>
+      </c>
+      <c r="H110" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="111" spans="7:8">
+      <c r="G111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="7:8">
+      <c r="G112" t="s">
+        <v>42</v>
+      </c>
+      <c r="H112" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8">
+      <c r="G113" t="s">
+        <v>42</v>
+      </c>
+      <c r="H113" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="7:8">
+      <c r="G114" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="115" spans="7:8">
+      <c r="G115" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="116" spans="7:8">
+      <c r="G116" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5571,7 +6054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -5609,7 +6092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update Notes and Tasks
</commit_message>
<xml_diff>
--- a/Support/ThemeTasks.xlsx
+++ b/Support/ThemeTasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesMc\Data\Clients\DigitalZenWorks\DigitalZenThemePrevious\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7997D0E2-B24B-4A0E-B048-CD4AB3515330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CAC6F-B963-4E83-B2C9-90E09C8A7A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1521,11 +1521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R198"/>
+  <dimension ref="A1:R197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1605,13 +1605,13 @@
         <v>199</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="L3" s="8">
         <v>43986</v>
@@ -1622,16 +1622,25 @@
         <v>199</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>217</v>
       </c>
+      <c r="E4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F4" t="s">
+        <v>371</v>
+      </c>
       <c r="G4" t="s">
-        <v>234</v>
-      </c>
-      <c r="L4" s="8">
-        <v>43986</v>
+        <v>372</v>
+      </c>
+      <c r="I4" t="s">
+        <v>373</v>
+      </c>
+      <c r="L4" s="1">
+        <v>44992</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1639,7 +1648,7 @@
         <v>199</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>217</v>
@@ -1647,14 +1656,8 @@
       <c r="E5" t="s">
         <v>366</v>
       </c>
-      <c r="F5" t="s">
-        <v>371</v>
-      </c>
       <c r="G5" t="s">
-        <v>372</v>
-      </c>
-      <c r="I5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="L5" s="1">
         <v>44992</v>
@@ -1665,7 +1668,7 @@
         <v>199</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>217</v>
@@ -1674,7 +1677,7 @@
         <v>366</v>
       </c>
       <c r="G6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L6" s="1">
         <v>44992</v>
@@ -1685,16 +1688,13 @@
         <v>199</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
       </c>
-      <c r="E7" t="s">
-        <v>366</v>
-      </c>
       <c r="G7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L7" s="1">
         <v>44992</v>
@@ -1705,16 +1705,16 @@
         <v>199</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>217</v>
       </c>
       <c r="G8" t="s">
-        <v>370</v>
+        <v>251</v>
       </c>
       <c r="L8" s="1">
-        <v>44992</v>
+        <v>43990</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1722,16 +1722,16 @@
         <v>199</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>217</v>
       </c>
       <c r="G9" t="s">
-        <v>251</v>
-      </c>
-      <c r="L9" s="1">
-        <v>43990</v>
+        <v>229</v>
+      </c>
+      <c r="L9" s="8">
+        <v>43986</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1739,13 +1739,16 @@
         <v>199</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>229</v>
+        <v>242</v>
+      </c>
+      <c r="H10" t="s">
+        <v>243</v>
       </c>
       <c r="L10" s="8">
         <v>43986</v>
@@ -1756,19 +1759,16 @@
         <v>199</v>
       </c>
       <c r="B11">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>217</v>
       </c>
       <c r="G11" t="s">
-        <v>242</v>
-      </c>
-      <c r="H11" t="s">
-        <v>243</v>
-      </c>
-      <c r="L11" s="8">
-        <v>43986</v>
+        <v>33</v>
+      </c>
+      <c r="L11" s="1">
+        <v>43712</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1776,13 +1776,13 @@
         <v>199</v>
       </c>
       <c r="B12">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>217</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="L12" s="1">
         <v>43712</v>
@@ -1793,13 +1793,13 @@
         <v>199</v>
       </c>
       <c r="B13">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
         <v>217</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="L13" s="1">
         <v>43712</v>
@@ -1810,16 +1810,16 @@
         <v>199</v>
       </c>
       <c r="B14">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>217</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>208</v>
       </c>
       <c r="L14" s="1">
-        <v>43712</v>
+        <v>43976</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1827,16 +1827,19 @@
         <v>199</v>
       </c>
       <c r="B15">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
         <v>217</v>
       </c>
+      <c r="E15" t="s">
+        <v>226</v>
+      </c>
       <c r="G15" t="s">
-        <v>208</v>
+        <v>29</v>
       </c>
       <c r="L15" s="1">
-        <v>43976</v>
+        <v>43712</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1844,7 +1847,7 @@
         <v>199</v>
       </c>
       <c r="B16">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
         <v>217</v>
@@ -1853,10 +1856,13 @@
         <v>226</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="L16" s="1">
-        <v>43712</v>
+        <v>43661</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1864,7 +1870,7 @@
         <v>199</v>
       </c>
       <c r="B17">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
         <v>217</v>
@@ -1873,21 +1879,18 @@
         <v>226</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="L17" s="1">
         <v>43661</v>
       </c>
-      <c r="M17" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>199</v>
       </c>
       <c r="B18">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
         <v>217</v>
@@ -1896,7 +1899,7 @@
         <v>226</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="L18" s="1">
         <v>43661</v>
@@ -1907,7 +1910,7 @@
         <v>199</v>
       </c>
       <c r="B19">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
         <v>217</v>
@@ -1916,7 +1919,7 @@
         <v>226</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L19" s="1">
         <v>43661</v>
@@ -1927,7 +1930,7 @@
         <v>199</v>
       </c>
       <c r="B20">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
         <v>217</v>
@@ -1936,7 +1939,7 @@
         <v>226</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="L20" s="1">
         <v>43661</v>
@@ -1947,19 +1950,19 @@
         <v>199</v>
       </c>
       <c r="B21">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
         <v>217</v>
       </c>
       <c r="E21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G21" t="s">
-        <v>228</v>
+        <v>30</v>
       </c>
       <c r="L21" s="1">
-        <v>43661</v>
+        <v>43660</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1967,7 +1970,7 @@
         <v>199</v>
       </c>
       <c r="B22">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
         <v>217</v>
@@ -1976,7 +1979,7 @@
         <v>227</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L22" s="1">
         <v>43660</v>
@@ -1987,7 +1990,7 @@
         <v>199</v>
       </c>
       <c r="B23">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
         <v>217</v>
@@ -1996,10 +1999,10 @@
         <v>227</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L23" s="1">
-        <v>43660</v>
+        <v>43712</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2007,7 +2010,7 @@
         <v>199</v>
       </c>
       <c r="B24">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
         <v>217</v>
@@ -2016,83 +2019,77 @@
         <v>227</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="L24" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25">
-        <v>147</v>
-      </c>
+        <v>43661</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75">
+      <c r="A25" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="5">
+        <v>150</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" t="s">
         <v>217</v>
       </c>
-      <c r="E25" t="s">
-        <v>227</v>
-      </c>
-      <c r="G25" t="s">
-        <v>228</v>
-      </c>
-      <c r="L25" s="1">
-        <v>43661</v>
-      </c>
+      <c r="E25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="2">
+        <v>42636</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:15" ht="15.75">
-      <c r="A26" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="5">
-        <v>150</v>
-      </c>
-      <c r="C26" s="5"/>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26">
+        <v>151</v>
+      </c>
       <c r="D26" t="s">
         <v>217</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="G26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="2">
-        <v>42636</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="1">
+        <v>43712</v>
+      </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>199</v>
       </c>
-      <c r="B27">
-        <v>151</v>
-      </c>
-      <c r="D27" t="s">
-        <v>217</v>
-      </c>
       <c r="G27" t="s">
-        <v>34</v>
+        <v>277</v>
       </c>
       <c r="L27" s="1">
-        <v>43712</v>
+        <v>44992</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>199</v>
       </c>
+      <c r="D28" t="s">
+        <v>217</v>
+      </c>
       <c r="G28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="L28" s="1">
         <v>44992</v>
@@ -2106,7 +2103,13 @@
         <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>272</v>
+        <v>306</v>
+      </c>
+      <c r="H29" t="s">
+        <v>307</v>
+      </c>
+      <c r="I29" t="s">
+        <v>308</v>
       </c>
       <c r="L29" s="1">
         <v>44992</v>
@@ -2120,7 +2123,7 @@
         <v>217</v>
       </c>
       <c r="G30" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="H30" t="s">
         <v>307</v>
@@ -2140,13 +2143,13 @@
         <v>217</v>
       </c>
       <c r="G31" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H31" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="I31" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="L31" s="1">
         <v>44992</v>
@@ -2160,12 +2163,9 @@
         <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H32" t="s">
-        <v>312</v>
-      </c>
-      <c r="I32" t="s">
         <v>313</v>
       </c>
       <c r="L32" s="1">
@@ -2180,10 +2180,13 @@
         <v>217</v>
       </c>
       <c r="G33" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H33" t="s">
-        <v>313</v>
+        <v>316</v>
+      </c>
+      <c r="I33" t="s">
+        <v>317</v>
       </c>
       <c r="L33" s="1">
         <v>44992</v>
@@ -2197,13 +2200,7 @@
         <v>217</v>
       </c>
       <c r="G34" t="s">
-        <v>315</v>
-      </c>
-      <c r="H34" t="s">
-        <v>316</v>
-      </c>
-      <c r="I34" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L34" s="1">
         <v>44992</v>
@@ -2217,7 +2214,7 @@
         <v>217</v>
       </c>
       <c r="G35" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="L35" s="1">
         <v>44992</v>
@@ -2231,7 +2228,7 @@
         <v>217</v>
       </c>
       <c r="G36" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="L36" s="1">
         <v>44992</v>
@@ -2245,7 +2242,7 @@
         <v>217</v>
       </c>
       <c r="G37" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="L37" s="1">
         <v>44992</v>
@@ -2259,7 +2256,7 @@
         <v>217</v>
       </c>
       <c r="G38" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="L38" s="1">
         <v>44992</v>
@@ -2273,7 +2270,7 @@
         <v>217</v>
       </c>
       <c r="G39" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L39" s="1">
         <v>44992</v>
@@ -2287,7 +2284,7 @@
         <v>217</v>
       </c>
       <c r="G40" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="L40" s="1">
         <v>44992</v>
@@ -2301,7 +2298,7 @@
         <v>217</v>
       </c>
       <c r="G41" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L41" s="1">
         <v>44992</v>
@@ -2315,7 +2312,7 @@
         <v>217</v>
       </c>
       <c r="G42" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L42" s="1">
         <v>44992</v>
@@ -2329,7 +2326,7 @@
         <v>217</v>
       </c>
       <c r="G43" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L43" s="1">
         <v>44992</v>
@@ -2343,7 +2340,7 @@
         <v>217</v>
       </c>
       <c r="G44" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L44" s="1">
         <v>44992</v>
@@ -2357,7 +2354,7 @@
         <v>217</v>
       </c>
       <c r="G45" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L45" s="1">
         <v>44992</v>
@@ -2371,7 +2368,7 @@
         <v>217</v>
       </c>
       <c r="G46" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L46" s="1">
         <v>44992</v>
@@ -2385,7 +2382,7 @@
         <v>217</v>
       </c>
       <c r="G47" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L47" s="1">
         <v>44992</v>
@@ -2399,7 +2396,7 @@
         <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>359</v>
+        <v>194</v>
       </c>
       <c r="L48" s="1">
         <v>44992</v>
@@ -2413,7 +2410,7 @@
         <v>217</v>
       </c>
       <c r="G49" t="s">
-        <v>194</v>
+        <v>360</v>
       </c>
       <c r="L49" s="1">
         <v>44992</v>
@@ -2427,7 +2424,7 @@
         <v>217</v>
       </c>
       <c r="G50" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="L50" s="1">
         <v>44992</v>
@@ -2435,13 +2432,16 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>94</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>217</v>
+        <v>342</v>
       </c>
       <c r="G51" t="s">
-        <v>361</v>
+        <v>274</v>
       </c>
       <c r="L51" s="1">
         <v>44992</v>
@@ -2452,13 +2452,13 @@
         <v>94</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G52" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L52" s="1">
         <v>44992</v>
@@ -2469,16 +2469,19 @@
         <v>94</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>341</v>
+        <v>219</v>
       </c>
       <c r="G53" t="s">
-        <v>271</v>
+        <v>20</v>
       </c>
       <c r="L53" s="1">
-        <v>44992</v>
+        <v>43660</v>
+      </c>
+      <c r="M53" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2486,19 +2489,16 @@
         <v>94</v>
       </c>
       <c r="B54">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D54" t="s">
         <v>219</v>
       </c>
       <c r="G54" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="L54" s="1">
-        <v>43660</v>
-      </c>
-      <c r="M54" t="s">
-        <v>21</v>
+        <v>43712</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2506,13 +2506,13 @@
         <v>94</v>
       </c>
       <c r="B55">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>219</v>
       </c>
       <c r="G55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L55" s="1">
         <v>43712</v>
@@ -2523,13 +2523,13 @@
         <v>94</v>
       </c>
       <c r="B56">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D56" t="s">
         <v>219</v>
       </c>
       <c r="G56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L56" s="1">
         <v>43712</v>
@@ -2540,13 +2540,13 @@
         <v>94</v>
       </c>
       <c r="B57">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D57" t="s">
         <v>219</v>
       </c>
       <c r="G57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L57" s="1">
         <v>43712</v>
@@ -2557,13 +2557,13 @@
         <v>94</v>
       </c>
       <c r="B58">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s">
         <v>219</v>
       </c>
       <c r="G58" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L58" s="1">
         <v>43712</v>
@@ -2574,13 +2574,13 @@
         <v>94</v>
       </c>
       <c r="B59">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
         <v>219</v>
       </c>
       <c r="G59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L59" s="1">
         <v>43712</v>
@@ -2591,13 +2591,13 @@
         <v>94</v>
       </c>
       <c r="B60">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
         <v>219</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L60" s="1">
         <v>43712</v>
@@ -2608,13 +2608,13 @@
         <v>94</v>
       </c>
       <c r="B61">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
         <v>219</v>
       </c>
       <c r="G61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L61" s="1">
         <v>43712</v>
@@ -2625,13 +2625,13 @@
         <v>94</v>
       </c>
       <c r="B62">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D62" t="s">
         <v>219</v>
       </c>
       <c r="G62" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="L62" s="1">
         <v>43712</v>
@@ -2642,57 +2642,66 @@
         <v>94</v>
       </c>
       <c r="B63">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D63" t="s">
         <v>219</v>
       </c>
       <c r="G63" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="L63" s="1">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+        <v>43665</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15.75">
       <c r="A64" t="s">
         <v>94</v>
       </c>
       <c r="B64">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D64" t="s">
         <v>219</v>
       </c>
       <c r="G64" t="s">
-        <v>66</v>
-      </c>
-      <c r="L64" s="1">
-        <v>43665</v>
+        <v>67</v>
+      </c>
+      <c r="H64" t="s">
+        <v>126</v>
+      </c>
+      <c r="L64" s="2">
+        <v>42636</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="15.75">
-      <c r="A65" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65">
-        <v>48</v>
-      </c>
+      <c r="A65" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
       <c r="D65" t="s">
         <v>219</v>
       </c>
-      <c r="G65" t="s">
-        <v>67</v>
-      </c>
-      <c r="H65" t="s">
-        <v>126</v>
-      </c>
+      <c r="E65" s="3"/>
+      <c r="G65" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J65" s="5"/>
       <c r="L65" s="2">
         <v>42636</v>
       </c>
       <c r="M65" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
     </row>
     <row r="66" spans="1:18" ht="15.75">
       <c r="A66" s="3" t="s">
@@ -2708,7 +2717,7 @@
         <v>108</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J66" s="5"/>
       <c r="L66" s="2">
@@ -2720,25 +2729,18 @@
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" spans="1:18" ht="15.75">
-      <c r="A67" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
+    <row r="67" spans="1:18">
+      <c r="A67" t="s">
+        <v>94</v>
+      </c>
       <c r="D67" t="s">
         <v>219</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="G67" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J67" s="5"/>
-      <c r="L67" s="2">
-        <v>42636</v>
+      <c r="G67" t="s">
+        <v>97</v>
+      </c>
+      <c r="L67" s="6">
+        <v>42754</v>
       </c>
       <c r="M67" s="5" t="s">
         <v>197</v>
@@ -2746,18 +2748,26 @@
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
     </row>
-    <row r="68" spans="1:18">
-      <c r="A68" t="s">
+    <row r="68" spans="1:18" ht="15.75">
+      <c r="A68" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
       <c r="D68" t="s">
         <v>219</v>
       </c>
-      <c r="G68" t="s">
-        <v>97</v>
-      </c>
-      <c r="L68" s="6">
-        <v>42754</v>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J68" s="5"/>
+      <c r="L68" s="2">
+        <v>42636</v>
       </c>
       <c r="M68" s="5" t="s">
         <v>197</v>
@@ -2765,42 +2775,32 @@
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
     </row>
-    <row r="69" spans="1:18" ht="15.75">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:18">
+      <c r="A69" t="s">
         <v>94</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
       <c r="D69" t="s">
         <v>219</v>
       </c>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J69" s="5"/>
-      <c r="L69" s="2">
-        <v>42636</v>
+      <c r="G69" t="s">
+        <v>140</v>
+      </c>
+      <c r="L69" s="1">
+        <v>43712</v>
       </c>
       <c r="M69" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-    </row>
-    <row r="70" spans="1:18">
-      <c r="A70" t="s">
+    </row>
+    <row r="70" spans="1:18" ht="15.75">
+      <c r="A70" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D70" t="s">
         <v>219</v>
       </c>
       <c r="G70" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="L70" s="1">
         <v>43712</v>
@@ -2810,93 +2810,99 @@
       </c>
     </row>
     <row r="71" spans="1:18" ht="15.75">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D71" t="s">
-        <v>219</v>
-      </c>
+      <c r="D71" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" t="s">
+        <v>105</v>
+      </c>
+      <c r="F71" s="5"/>
       <c r="G71" t="s">
-        <v>151</v>
-      </c>
-      <c r="L71" s="1">
-        <v>43712</v>
+        <v>116</v>
+      </c>
+      <c r="H71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="6">
+        <v>42754</v>
       </c>
       <c r="M71" s="5" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" ht="15.75">
-      <c r="A72" s="3" t="s">
+      <c r="O71" s="3"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="A72" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
       <c r="D72" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E72" t="s">
-        <v>105</v>
-      </c>
+      <c r="E72" s="5"/>
       <c r="F72" s="5"/>
-      <c r="G72" t="s">
-        <v>116</v>
+      <c r="G72" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
       <c r="L72" s="6">
-        <v>42754</v>
+        <v>42556</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="O72" s="3"/>
-      <c r="P72" s="2"/>
-      <c r="Q72" s="3"/>
-      <c r="R72" s="3"/>
-    </row>
-    <row r="73" spans="1:18">
-      <c r="A73" s="5" t="s">
+    </row>
+    <row r="73" spans="1:18" ht="15.75">
+      <c r="A73" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
       <c r="D73" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E73" s="5"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="G73" t="s">
+        <v>117</v>
+      </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="L73" s="6">
-        <v>42556</v>
+        <v>42754</v>
       </c>
       <c r="M73" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="15.75">
-      <c r="A74" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F74" s="5"/>
+    <row r="74" spans="1:18">
+      <c r="A74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>218</v>
+      </c>
       <c r="G74" t="s">
-        <v>117</v>
-      </c>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="6">
-        <v>42754</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
+      </c>
+      <c r="H74" t="s">
+        <v>204</v>
+      </c>
+      <c r="L74" s="1">
+        <v>43660</v>
+      </c>
+      <c r="M74" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:18">
@@ -2904,16 +2910,13 @@
         <v>119</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
         <v>218</v>
       </c>
       <c r="G75" t="s">
-        <v>203</v>
-      </c>
-      <c r="H75" t="s">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="L75" s="1">
         <v>43660</v>
@@ -2927,19 +2930,16 @@
         <v>119</v>
       </c>
       <c r="B76">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
         <v>218</v>
       </c>
       <c r="G76" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L76" s="1">
         <v>43660</v>
-      </c>
-      <c r="M76" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:18">
@@ -2947,16 +2947,19 @@
         <v>119</v>
       </c>
       <c r="B77">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="D77" t="s">
         <v>218</v>
       </c>
       <c r="G77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L77" s="1">
-        <v>43660</v>
+        <v>43661</v>
+      </c>
+      <c r="M77" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -2964,76 +2967,70 @@
         <v>119</v>
       </c>
       <c r="B78">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D78" t="s">
         <v>218</v>
       </c>
       <c r="G78" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L78" s="1">
         <v>43661</v>
       </c>
-      <c r="M78" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
-      <c r="A79" t="s">
+    </row>
+    <row r="79" spans="1:18" ht="15.75">
+      <c r="A79" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B79">
-        <v>149</v>
-      </c>
+      <c r="C79" s="5"/>
       <c r="D79" t="s">
         <v>218</v>
       </c>
       <c r="G79" t="s">
-        <v>44</v>
-      </c>
-      <c r="L79" s="1">
-        <v>43661</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" ht="15.75">
-      <c r="A80" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L79" s="6">
+        <v>42754</v>
+      </c>
+      <c r="M79" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="A80" t="s">
         <v>119</v>
       </c>
+      <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" t="s">
         <v>218</v>
       </c>
       <c r="G80" t="s">
-        <v>99</v>
-      </c>
-      <c r="L80" s="6">
-        <v>42754</v>
-      </c>
-      <c r="M80" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="N80" s="5"/>
+        <v>230</v>
+      </c>
+      <c r="H80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="8">
+        <v>43986</v>
+      </c>
       <c r="O80" s="5"/>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>119</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
       <c r="D81" t="s">
         <v>218</v>
       </c>
       <c r="G81" t="s">
-        <v>230</v>
-      </c>
-      <c r="H81" s="5"/>
-      <c r="K81" s="5"/>
+        <v>236</v>
+      </c>
       <c r="L81" s="8">
         <v>43986</v>
       </c>
-      <c r="O81" s="5"/>
     </row>
     <row r="82" spans="1:15">
       <c r="A82" t="s">
@@ -3043,7 +3040,7 @@
         <v>218</v>
       </c>
       <c r="G82" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L82" s="8">
         <v>43986</v>
@@ -3057,7 +3054,7 @@
         <v>218</v>
       </c>
       <c r="G83" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L83" s="8">
         <v>43986</v>
@@ -3071,7 +3068,7 @@
         <v>218</v>
       </c>
       <c r="G84" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L84" s="8">
         <v>43986</v>
@@ -3085,7 +3082,7 @@
         <v>218</v>
       </c>
       <c r="G85" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L85" s="8">
         <v>43986</v>
@@ -3099,57 +3096,75 @@
         <v>218</v>
       </c>
       <c r="G86" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="L86" s="8">
         <v>43986</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
-      <c r="A87" t="s">
-        <v>119</v>
+    <row r="87" spans="1:15" ht="15.75">
+      <c r="A87" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>218</v>
-      </c>
-      <c r="G87" t="s">
-        <v>245</v>
-      </c>
-      <c r="L87" s="8">
-        <v>43986</v>
+        <v>205</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H87" s="3"/>
+      <c r="L87" s="2">
+        <v>42535</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="15.75">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B88">
-        <v>3</v>
-      </c>
+      <c r="B88" s="3">
+        <v>14</v>
+      </c>
+      <c r="C88" s="3"/>
       <c r="D88" t="s">
         <v>205</v>
       </c>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
+      <c r="E88" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F88" s="3"/>
       <c r="G88" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H88" s="3"/>
-      <c r="L88" s="2">
-        <v>42535</v>
+        <v>130</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="7">
+        <v>42071</v>
       </c>
       <c r="M88" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="O88" s="5"/>
     </row>
     <row r="89" spans="1:15" ht="15.75">
       <c r="A89" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B89" s="3">
-        <v>14</v>
-      </c>
-      <c r="C89" s="3"/>
+      <c r="B89" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="C89" s="4"/>
       <c r="D89" t="s">
         <v>205</v>
       </c>
@@ -3157,17 +3172,15 @@
         <v>201</v>
       </c>
       <c r="F89" s="3"/>
-      <c r="G89" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>129</v>
-      </c>
+      <c r="G89" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H89" s="4"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="7">
-        <v>42071</v>
+        <v>41513</v>
       </c>
       <c r="M89" s="5" t="s">
         <v>197</v>
@@ -3175,33 +3188,30 @@
       <c r="O89" s="5"/>
     </row>
     <row r="90" spans="1:15" ht="15.75">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B90" s="4">
-        <v>15.4</v>
-      </c>
-      <c r="C90" s="4"/>
+      <c r="B90" s="5">
+        <v>32</v>
+      </c>
+      <c r="C90" s="5"/>
       <c r="D90" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F90" s="3"/>
-      <c r="G90" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H90" s="4"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="7">
-        <v>41513</v>
+      <c r="G90" t="s">
+        <v>104</v>
+      </c>
+      <c r="H90" t="s">
+        <v>106</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="L90" s="2">
+        <v>42636</v>
       </c>
       <c r="M90" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="N90" s="5"/>
       <c r="O90" s="5"/>
     </row>
     <row r="91" spans="1:15" ht="15.75">
@@ -3209,17 +3219,18 @@
         <v>200</v>
       </c>
       <c r="B91" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" t="s">
         <v>205</v>
       </c>
-      <c r="G91" t="s">
+      <c r="E91" s="3"/>
+      <c r="G91" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="H91" t="s">
-        <v>106</v>
+      <c r="H91" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="J91" s="5"/>
       <c r="L91" s="2">
@@ -3231,27 +3242,22 @@
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
     </row>
-    <row r="92" spans="1:15" ht="15.75">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:15">
+      <c r="A92" t="s">
         <v>200</v>
       </c>
-      <c r="B92" s="5">
-        <v>33</v>
-      </c>
-      <c r="C92" s="5"/>
+      <c r="B92">
+        <v>49</v>
+      </c>
       <c r="D92" t="s">
         <v>205</v>
       </c>
-      <c r="E92" s="3"/>
-      <c r="G92" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>103</v>
+      <c r="G92" t="s">
+        <v>98</v>
       </c>
       <c r="J92" s="5"/>
-      <c r="L92" s="2">
-        <v>42636</v>
+      <c r="L92" s="6">
+        <v>42754</v>
       </c>
       <c r="M92" s="5" t="s">
         <v>197</v>
@@ -3264,46 +3270,49 @@
         <v>200</v>
       </c>
       <c r="B93">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D93" t="s">
         <v>205</v>
       </c>
       <c r="G93" t="s">
-        <v>98</v>
-      </c>
-      <c r="J93" s="5"/>
-      <c r="L93" s="6">
-        <v>42754</v>
+        <v>137</v>
+      </c>
+      <c r="H93" t="s">
+        <v>138</v>
+      </c>
+      <c r="L93" s="1">
+        <v>43712</v>
       </c>
       <c r="M93" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N93" s="5"/>
-      <c r="O93" s="5"/>
-    </row>
-    <row r="94" spans="1:15">
-      <c r="A94" t="s">
+    </row>
+    <row r="94" spans="1:15" ht="15.75">
+      <c r="A94" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B94">
-        <v>50</v>
-      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
       <c r="D94" t="s">
         <v>205</v>
       </c>
+      <c r="E94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F94" s="5"/>
       <c r="G94" t="s">
-        <v>137</v>
-      </c>
-      <c r="H94" t="s">
-        <v>138</v>
-      </c>
-      <c r="L94" s="1">
-        <v>43712</v>
+        <v>89</v>
+      </c>
+      <c r="J94" s="5"/>
+      <c r="L94" s="2">
+        <v>42636</v>
       </c>
       <c r="M94" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
     </row>
     <row r="95" spans="1:15" ht="15.75">
       <c r="A95" s="3" t="s">
@@ -3319,7 +3328,7 @@
       </c>
       <c r="F95" s="5"/>
       <c r="G95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J95" s="5"/>
       <c r="L95" s="2">
@@ -3345,7 +3354,7 @@
       </c>
       <c r="F96" s="5"/>
       <c r="G96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J96" s="5"/>
       <c r="L96" s="2">
@@ -3366,12 +3375,12 @@
       <c r="D97" t="s">
         <v>205</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F97" s="5"/>
-      <c r="G97" t="s">
-        <v>87</v>
+      <c r="G97" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="J97" s="5"/>
       <c r="L97" s="2">
@@ -3383,30 +3392,24 @@
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
     </row>
-    <row r="98" spans="1:15" ht="15.75">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:15">
+      <c r="A98" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
       <c r="D98" t="s">
         <v>205</v>
       </c>
-      <c r="E98" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F98" s="5"/>
-      <c r="G98" s="3" t="s">
-        <v>85</v>
+      <c r="G98" t="s">
+        <v>125</v>
       </c>
       <c r="J98" s="5"/>
-      <c r="L98" s="2">
-        <v>42636</v>
+      <c r="K98" s="5"/>
+      <c r="L98" s="6">
+        <v>42754</v>
       </c>
       <c r="M98" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N98" s="5"/>
       <c r="O98" s="5"/>
     </row>
     <row r="99" spans="1:15">
@@ -3417,27 +3420,24 @@
         <v>205</v>
       </c>
       <c r="G99" t="s">
-        <v>125</v>
-      </c>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="6">
-        <v>42754</v>
+        <v>146</v>
+      </c>
+      <c r="L99" s="1">
+        <v>43712</v>
       </c>
       <c r="M99" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="O99" s="5"/>
-    </row>
-    <row r="100" spans="1:15">
-      <c r="A100" t="s">
+    </row>
+    <row r="100" spans="1:15" ht="15.75">
+      <c r="A100" s="4" t="s">
         <v>200</v>
       </c>
       <c r="D100" t="s">
         <v>205</v>
       </c>
       <c r="G100" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L100" s="1">
         <v>43712</v>
@@ -3446,15 +3446,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15.75">
-      <c r="A101" s="4" t="s">
+    <row r="101" spans="1:15">
+      <c r="A101" t="s">
         <v>200</v>
       </c>
       <c r="D101" t="s">
         <v>205</v>
       </c>
       <c r="G101" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L101" s="1">
         <v>43712</v>
@@ -3463,15 +3463,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
-      <c r="A102" t="s">
+    <row r="102" spans="1:15" ht="15.75">
+      <c r="A102" s="4" t="s">
         <v>200</v>
       </c>
       <c r="D102" t="s">
         <v>205</v>
       </c>
       <c r="G102" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L102" s="1">
         <v>43712</v>
@@ -3480,15 +3480,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="15.75">
-      <c r="A103" s="4" t="s">
+    <row r="103" spans="1:15">
+      <c r="A103" t="s">
         <v>200</v>
       </c>
       <c r="D103" t="s">
         <v>205</v>
       </c>
       <c r="G103" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L103" s="1">
         <v>43712</v>
@@ -3505,7 +3505,7 @@
         <v>205</v>
       </c>
       <c r="G104" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L104" s="1">
         <v>43712</v>
@@ -3514,15 +3514,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
-      <c r="A105" t="s">
+    <row r="105" spans="1:15" ht="15.75">
+      <c r="A105" s="4" t="s">
         <v>200</v>
       </c>
       <c r="D105" t="s">
         <v>205</v>
       </c>
       <c r="G105" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L105" s="1">
         <v>43712</v>
@@ -3531,15 +3531,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="15.75">
-      <c r="A106" s="4" t="s">
+    <row r="106" spans="1:15">
+      <c r="A106" t="s">
         <v>200</v>
       </c>
       <c r="D106" t="s">
         <v>205</v>
       </c>
       <c r="G106" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L106" s="1">
         <v>43712</v>
@@ -3556,7 +3556,7 @@
         <v>205</v>
       </c>
       <c r="G107" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L107" s="1">
         <v>43712</v>
@@ -3573,7 +3573,7 @@
         <v>205</v>
       </c>
       <c r="G108" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L108" s="1">
         <v>43712</v>
@@ -3590,7 +3590,7 @@
         <v>205</v>
       </c>
       <c r="G109" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L109" s="1">
         <v>43712</v>
@@ -3607,7 +3607,7 @@
         <v>205</v>
       </c>
       <c r="G110" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L110" s="1">
         <v>43712</v>
@@ -3624,7 +3624,7 @@
         <v>205</v>
       </c>
       <c r="G111" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L111" s="1">
         <v>43712</v>
@@ -3641,7 +3641,7 @@
         <v>205</v>
       </c>
       <c r="G112" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L112" s="1">
         <v>43712</v>
@@ -3658,7 +3658,7 @@
         <v>205</v>
       </c>
       <c r="G113" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L113" s="1">
         <v>43712</v>
@@ -3675,7 +3675,7 @@
         <v>205</v>
       </c>
       <c r="G114" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L114" s="1">
         <v>43712</v>
@@ -3692,7 +3692,7 @@
         <v>205</v>
       </c>
       <c r="G115" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L115" s="1">
         <v>43712</v>
@@ -3709,7 +3709,7 @@
         <v>205</v>
       </c>
       <c r="G116" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L116" s="1">
         <v>43712</v>
@@ -3726,7 +3726,7 @@
         <v>205</v>
       </c>
       <c r="G117" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L117" s="1">
         <v>43712</v>
@@ -3743,7 +3743,7 @@
         <v>205</v>
       </c>
       <c r="G118" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L118" s="1">
         <v>43712</v>
@@ -3760,7 +3760,7 @@
         <v>205</v>
       </c>
       <c r="G119" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L119" s="1">
         <v>43712</v>
@@ -3777,7 +3777,7 @@
         <v>205</v>
       </c>
       <c r="G120" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L120" s="1">
         <v>43712</v>
@@ -3794,7 +3794,7 @@
         <v>205</v>
       </c>
       <c r="G121" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L121" s="1">
         <v>43712</v>
@@ -3811,7 +3811,7 @@
         <v>205</v>
       </c>
       <c r="G122" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L122" s="1">
         <v>43712</v>
@@ -3828,7 +3828,7 @@
         <v>205</v>
       </c>
       <c r="G123" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L123" s="1">
         <v>43712</v>
@@ -3845,7 +3845,7 @@
         <v>205</v>
       </c>
       <c r="G124" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L124" s="1">
         <v>43712</v>
@@ -3862,7 +3862,10 @@
         <v>205</v>
       </c>
       <c r="G125" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="H125" t="s">
+        <v>176</v>
       </c>
       <c r="L125" s="1">
         <v>43712</v>
@@ -3879,10 +3882,10 @@
         <v>205</v>
       </c>
       <c r="G126" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H126" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L126" s="1">
         <v>43712</v>
@@ -3899,10 +3902,10 @@
         <v>205</v>
       </c>
       <c r="G127" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H127" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L127" s="1">
         <v>43712</v>
@@ -3919,10 +3922,10 @@
         <v>205</v>
       </c>
       <c r="G128" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H128" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L128" s="1">
         <v>43712</v>
@@ -3939,10 +3942,10 @@
         <v>205</v>
       </c>
       <c r="G129" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H129" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L129" s="1">
         <v>43712</v>
@@ -3959,10 +3962,10 @@
         <v>205</v>
       </c>
       <c r="G130" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H130" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L130" s="1">
         <v>43712</v>
@@ -3979,10 +3982,10 @@
         <v>205</v>
       </c>
       <c r="G131" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H131" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L131" s="1">
         <v>43712</v>
@@ -3999,10 +4002,7 @@
         <v>205</v>
       </c>
       <c r="G132" t="s">
-        <v>187</v>
-      </c>
-      <c r="H132" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L132" s="1">
         <v>43712</v>
@@ -4019,7 +4019,7 @@
         <v>205</v>
       </c>
       <c r="G133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L133" s="1">
         <v>43712</v>
@@ -4036,7 +4036,7 @@
         <v>205</v>
       </c>
       <c r="G134" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L134" s="1">
         <v>43712</v>
@@ -4053,7 +4053,7 @@
         <v>205</v>
       </c>
       <c r="G135" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L135" s="1">
         <v>43712</v>
@@ -4070,7 +4070,7 @@
         <v>205</v>
       </c>
       <c r="G136" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L136" s="1">
         <v>43712</v>
@@ -4087,7 +4087,7 @@
         <v>205</v>
       </c>
       <c r="G137" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L137" s="1">
         <v>43712</v>
@@ -4104,7 +4104,7 @@
         <v>205</v>
       </c>
       <c r="G138" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L138" s="1">
         <v>43712</v>
@@ -4121,7 +4121,7 @@
         <v>205</v>
       </c>
       <c r="G139" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L139" s="1">
         <v>43712</v>
@@ -4130,166 +4130,166 @@
         <v>197</v>
       </c>
     </row>
-    <row r="140" spans="1:15">
-      <c r="A140" t="s">
+    <row r="140" spans="1:15" ht="15.75">
+      <c r="A140" s="3" t="s">
         <v>200</v>
       </c>
       <c r="D140" t="s">
         <v>205</v>
       </c>
       <c r="G140" t="s">
-        <v>196</v>
-      </c>
-      <c r="L140" s="1">
-        <v>43712</v>
+        <v>101</v>
+      </c>
+      <c r="H140" t="s">
+        <v>100</v>
+      </c>
+      <c r="K140" s="5"/>
+      <c r="L140" s="6">
+        <v>42754</v>
       </c>
       <c r="M140" s="5" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" ht="15.75">
-      <c r="A141" s="3" t="s">
+      <c r="N140" s="5"/>
+      <c r="O140" s="5"/>
+    </row>
+    <row r="141" spans="1:15">
+      <c r="A141" t="s">
         <v>200</v>
       </c>
       <c r="D141" t="s">
         <v>205</v>
       </c>
       <c r="G141" t="s">
-        <v>101</v>
-      </c>
-      <c r="H141" t="s">
-        <v>100</v>
-      </c>
-      <c r="K141" s="5"/>
-      <c r="L141" s="6">
-        <v>42754</v>
-      </c>
-      <c r="M141" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="N141" s="5"/>
-      <c r="O141" s="5"/>
-    </row>
-    <row r="142" spans="1:15">
-      <c r="A142" t="s">
-        <v>200</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="L141" s="8">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="15.75">
+      <c r="A142" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B142" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="C142" s="4"/>
       <c r="D142" t="s">
-        <v>205</v>
-      </c>
-      <c r="G142" t="s">
-        <v>233</v>
-      </c>
-      <c r="L142" s="8">
-        <v>43986</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E142" s="4"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H142" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="7">
+        <v>41513</v>
+      </c>
+      <c r="M142" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="O142" s="5"/>
     </row>
     <row r="143" spans="1:15" ht="15.75">
       <c r="A143" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B143" s="4">
-        <v>15.4</v>
-      </c>
-      <c r="C143" s="4"/>
+      <c r="B143" s="3">
+        <v>20</v>
+      </c>
+      <c r="C143" s="3"/>
       <c r="D143" t="s">
         <v>221</v>
       </c>
       <c r="E143" s="4"/>
       <c r="F143" s="3"/>
-      <c r="G143" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H143" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I143" s="3"/>
+      <c r="G143" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H143" s="3"/>
+      <c r="I143" s="3">
+        <v>5</v>
+      </c>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
       <c r="L143" s="7">
-        <v>41513</v>
+        <v>41452</v>
       </c>
       <c r="M143" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="O143" s="5"/>
     </row>
     <row r="144" spans="1:15" ht="15.75">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B144" s="3">
-        <v>20</v>
+      <c r="B144">
+        <v>21</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" t="s">
         <v>221</v>
       </c>
-      <c r="E144" s="4"/>
-      <c r="F144" s="3"/>
+      <c r="E144" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="G144" s="3" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="H144" s="3"/>
-      <c r="I144" s="3">
-        <v>5</v>
-      </c>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
-      <c r="L144" s="7">
-        <v>41452</v>
+      <c r="L144" s="2">
+        <v>42404</v>
       </c>
       <c r="M144" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3"/>
     </row>
     <row r="145" spans="1:15" ht="15.75">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="4" t="s">
         <v>223</v>
       </c>
       <c r="B145">
-        <v>21</v>
-      </c>
-      <c r="C145" s="3"/>
+        <v>30</v>
+      </c>
       <c r="D145" t="s">
         <v>221</v>
       </c>
-      <c r="E145" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G145" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H145" s="3"/>
-      <c r="J145" s="3"/>
-      <c r="K145" s="3"/>
-      <c r="L145" s="2">
-        <v>42404</v>
+      <c r="G145" t="s">
+        <v>139</v>
+      </c>
+      <c r="L145" s="1">
+        <v>43712</v>
       </c>
       <c r="M145" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N145" s="3"/>
-      <c r="O145" s="3"/>
-    </row>
-    <row r="146" spans="1:15" ht="15.75">
-      <c r="A146" s="4" t="s">
+    </row>
+    <row r="146" spans="1:15">
+      <c r="A146" t="s">
         <v>223</v>
       </c>
       <c r="B146">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D146" t="s">
         <v>221</v>
       </c>
       <c r="G146" t="s">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="L146" s="1">
-        <v>43712</v>
-      </c>
-      <c r="M146" s="5" t="s">
-        <v>197</v>
+        <v>43719</v>
       </c>
     </row>
     <row r="147" spans="1:15">
@@ -4297,120 +4297,125 @@
         <v>223</v>
       </c>
       <c r="B147">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="D147" t="s">
         <v>221</v>
       </c>
       <c r="G147" t="s">
-        <v>198</v>
+        <v>22</v>
       </c>
       <c r="L147" s="1">
-        <v>43719</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15">
-      <c r="A148" t="s">
+        <v>43661</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="15.75">
+      <c r="A148" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B148">
-        <v>150</v>
-      </c>
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
       <c r="D148" t="s">
         <v>221</v>
       </c>
-      <c r="G148" t="s">
-        <v>22</v>
-      </c>
-      <c r="L148" s="1">
-        <v>43661</v>
-      </c>
+      <c r="E148" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="5"/>
+      <c r="L148" s="2">
+        <v>42636</v>
+      </c>
+      <c r="M148" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="O148" s="5"/>
     </row>
     <row r="149" spans="1:15" ht="15.75">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B149" s="5"/>
-      <c r="C149" s="5"/>
       <c r="D149" t="s">
         <v>221</v>
       </c>
-      <c r="E149" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F149" s="3"/>
-      <c r="G149" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H149" s="3"/>
-      <c r="J149" s="3"/>
-      <c r="K149" s="5"/>
-      <c r="L149" s="2">
-        <v>42636</v>
+      <c r="G149" t="s">
+        <v>145</v>
+      </c>
+      <c r="L149" s="1">
+        <v>43712</v>
       </c>
       <c r="M149" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="O149" s="5"/>
     </row>
     <row r="150" spans="1:15" ht="15.75">
       <c r="A150" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
       <c r="D150" t="s">
         <v>221</v>
       </c>
-      <c r="G150" t="s">
-        <v>145</v>
-      </c>
-      <c r="L150" s="1">
-        <v>43712</v>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H150" s="4"/>
+      <c r="I150" s="4">
+        <v>30</v>
+      </c>
+      <c r="J150" s="4"/>
+      <c r="K150" s="4"/>
+      <c r="L150" s="7">
+        <v>41499</v>
       </c>
       <c r="M150" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="15.75">
-      <c r="A151" s="4" t="s">
+    <row r="151" spans="1:15">
+      <c r="A151" t="s">
         <v>223</v>
       </c>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
       <c r="D151" t="s">
         <v>221</v>
       </c>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H151" s="4"/>
-      <c r="I151" s="4">
-        <v>30</v>
-      </c>
-      <c r="J151" s="4"/>
-      <c r="K151" s="4"/>
-      <c r="L151" s="7">
-        <v>41499</v>
-      </c>
-      <c r="M151" s="5" t="s">
-        <v>197</v>
-      </c>
+      <c r="G151" t="s">
+        <v>206</v>
+      </c>
+      <c r="L151" s="1">
+        <v>43719</v>
+      </c>
+      <c r="M151" s="5"/>
+      <c r="N151" s="5"/>
+      <c r="O151" s="5"/>
     </row>
     <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>223</v>
       </c>
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
       <c r="D152" t="s">
         <v>221</v>
       </c>
       <c r="G152" t="s">
-        <v>206</v>
-      </c>
-      <c r="L152" s="1">
-        <v>43719</v>
-      </c>
-      <c r="M152" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="J152" s="5"/>
+      <c r="L152" s="8">
+        <v>42636</v>
+      </c>
+      <c r="M152" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="N152" s="5"/>
       <c r="O152" s="5"/>
     </row>
@@ -4418,17 +4423,15 @@
       <c r="A153" t="s">
         <v>223</v>
       </c>
-      <c r="B153" s="5"/>
-      <c r="C153" s="5"/>
       <c r="D153" t="s">
         <v>221</v>
       </c>
       <c r="G153" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J153" s="5"/>
-      <c r="L153" s="8">
-        <v>42636</v>
+      <c r="L153" s="6">
+        <v>42754</v>
       </c>
       <c r="M153" s="5" t="s">
         <v>197</v>
@@ -4440,15 +4443,17 @@
       <c r="A154" t="s">
         <v>223</v>
       </c>
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
       <c r="D154" t="s">
         <v>221</v>
       </c>
       <c r="G154" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J154" s="5"/>
-      <c r="L154" s="6">
-        <v>42754</v>
+      <c r="L154" s="8">
+        <v>42636</v>
       </c>
       <c r="M154" s="5" t="s">
         <v>197</v>
@@ -4465,10 +4470,12 @@
       <c r="D155" t="s">
         <v>221</v>
       </c>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
       <c r="G155" t="s">
-        <v>95</v>
-      </c>
-      <c r="J155" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="K155" s="5"/>
       <c r="L155" s="8">
         <v>42636</v>
       </c>
@@ -4482,24 +4489,21 @@
       <c r="A156" t="s">
         <v>223</v>
       </c>
-      <c r="B156" s="5"/>
-      <c r="C156" s="5"/>
       <c r="D156" t="s">
         <v>221</v>
       </c>
-      <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" t="s">
-        <v>90</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="J156" s="5"/>
       <c r="K156" s="5"/>
-      <c r="L156" s="8">
-        <v>42636</v>
+      <c r="L156" s="6">
+        <v>42754</v>
       </c>
       <c r="M156" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N156" s="5"/>
       <c r="O156" s="5"/>
     </row>
     <row r="157" spans="1:15">
@@ -4509,19 +4513,15 @@
       <c r="D157" t="s">
         <v>221</v>
       </c>
-      <c r="F157" s="5"/>
       <c r="G157" t="s">
-        <v>124</v>
-      </c>
-      <c r="J157" s="5"/>
-      <c r="K157" s="5"/>
-      <c r="L157" s="6">
-        <v>42754</v>
+        <v>141</v>
+      </c>
+      <c r="L157" s="1">
+        <v>43712</v>
       </c>
       <c r="M157" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="O157" s="5"/>
     </row>
     <row r="158" spans="1:15">
       <c r="A158" t="s">
@@ -4531,7 +4531,7 @@
         <v>221</v>
       </c>
       <c r="G158" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L158" s="1">
         <v>43712</v>
@@ -4548,14 +4548,13 @@
         <v>221</v>
       </c>
       <c r="G159" t="s">
-        <v>142</v>
-      </c>
-      <c r="L159" s="1">
-        <v>43712</v>
-      </c>
-      <c r="M159" s="5" t="s">
-        <v>197</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="L159" s="8">
+        <v>43986</v>
+      </c>
+      <c r="M159" s="5"/>
+      <c r="O159" s="5"/>
     </row>
     <row r="160" spans="1:15">
       <c r="A160" t="s">
@@ -4565,15 +4564,14 @@
         <v>221</v>
       </c>
       <c r="G160" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L160" s="8">
         <v>43986</v>
       </c>
-      <c r="M160" s="5"/>
       <c r="O160" s="5"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:13">
       <c r="A161" t="s">
         <v>223</v>
       </c>
@@ -4581,14 +4579,13 @@
         <v>221</v>
       </c>
       <c r="G161" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="L161" s="8">
         <v>43986</v>
       </c>
-      <c r="O161" s="5"/>
-    </row>
-    <row r="162" spans="1:15">
+    </row>
+    <row r="162" spans="1:13">
       <c r="A162" t="s">
         <v>223</v>
       </c>
@@ -4596,13 +4593,13 @@
         <v>221</v>
       </c>
       <c r="G162" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L162" s="8">
         <v>43986</v>
       </c>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:13">
       <c r="A163" t="s">
         <v>223</v>
       </c>
@@ -4610,13 +4607,13 @@
         <v>221</v>
       </c>
       <c r="G163" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L163" s="8">
         <v>43986</v>
       </c>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:13">
       <c r="A164" t="s">
         <v>223</v>
       </c>
@@ -4624,13 +4621,13 @@
         <v>221</v>
       </c>
       <c r="G164" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L164" s="8">
         <v>43986</v>
       </c>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:13">
       <c r="A165" t="s">
         <v>223</v>
       </c>
@@ -4638,13 +4635,13 @@
         <v>221</v>
       </c>
       <c r="G165" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L165" s="8">
         <v>43986</v>
       </c>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:13">
       <c r="A166" t="s">
         <v>223</v>
       </c>
@@ -4652,13 +4649,13 @@
         <v>221</v>
       </c>
       <c r="G166" t="s">
-        <v>249</v>
-      </c>
-      <c r="L166" s="8">
-        <v>43986</v>
-      </c>
-    </row>
-    <row r="167" spans="1:15">
+        <v>301</v>
+      </c>
+      <c r="L166" s="1">
+        <v>44992</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13">
       <c r="A167" t="s">
         <v>223</v>
       </c>
@@ -4666,13 +4663,13 @@
         <v>221</v>
       </c>
       <c r="G167" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="L167" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:13">
       <c r="A168" t="s">
         <v>223</v>
       </c>
@@ -4680,13 +4677,13 @@
         <v>221</v>
       </c>
       <c r="G168" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L168" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:13">
       <c r="A169" t="s">
         <v>223</v>
       </c>
@@ -4694,13 +4691,13 @@
         <v>221</v>
       </c>
       <c r="G169" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="L169" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:13">
       <c r="A170" t="s">
         <v>223</v>
       </c>
@@ -4708,13 +4705,16 @@
         <v>221</v>
       </c>
       <c r="G170" t="s">
-        <v>319</v>
+        <v>320</v>
+      </c>
+      <c r="H170" t="s">
+        <v>321</v>
       </c>
       <c r="L170" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:13">
       <c r="A171" t="s">
         <v>223</v>
       </c>
@@ -4722,16 +4722,13 @@
         <v>221</v>
       </c>
       <c r="G171" t="s">
-        <v>320</v>
-      </c>
-      <c r="H171" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L171" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:13">
       <c r="A172" t="s">
         <v>223</v>
       </c>
@@ -4739,13 +4736,13 @@
         <v>221</v>
       </c>
       <c r="G172" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="L172" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:13">
       <c r="A173" t="s">
         <v>223</v>
       </c>
@@ -4753,13 +4750,16 @@
         <v>221</v>
       </c>
       <c r="G173" t="s">
-        <v>325</v>
+        <v>346</v>
+      </c>
+      <c r="H173" t="s">
+        <v>347</v>
       </c>
       <c r="L173" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:13">
       <c r="A174" t="s">
         <v>223</v>
       </c>
@@ -4767,30 +4767,30 @@
         <v>221</v>
       </c>
       <c r="G174" t="s">
-        <v>346</v>
-      </c>
-      <c r="H174" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L174" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:13">
       <c r="A175" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D175" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G175" t="s">
-        <v>348</v>
+        <v>144</v>
       </c>
       <c r="L175" s="1">
-        <v>44992</v>
-      </c>
-    </row>
-    <row r="176" spans="1:15">
+        <v>43712</v>
+      </c>
+      <c r="M175" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13">
       <c r="A176" t="s">
         <v>222</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>220</v>
       </c>
       <c r="G176" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L176" s="1">
         <v>43712</v>
@@ -4809,54 +4809,41 @@
     </row>
     <row r="177" spans="1:15">
       <c r="A177" t="s">
-        <v>222</v>
+        <v>343</v>
       </c>
       <c r="D177" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G177" t="s">
-        <v>143</v>
+        <v>302</v>
       </c>
       <c r="L177" s="1">
-        <v>43712</v>
-      </c>
-      <c r="M177" s="5" t="s">
-        <v>197</v>
+        <v>44992</v>
       </c>
     </row>
     <row r="178" spans="1:15">
       <c r="A178" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D178" t="s">
-        <v>218</v>
+        <v>332</v>
       </c>
       <c r="G178" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="L178" s="1">
         <v>44992</v>
       </c>
     </row>
-    <row r="179" spans="1:15">
-      <c r="A179" t="s">
-        <v>345</v>
-      </c>
-      <c r="D179" t="s">
-        <v>332</v>
-      </c>
-      <c r="G179" t="s">
-        <v>344</v>
-      </c>
-      <c r="L179" s="1">
-        <v>44992</v>
-      </c>
-    </row>
-    <row r="183" spans="1:15">
-      <c r="O183" s="5"/>
-    </row>
-    <row r="191" spans="1:15">
-      <c r="L191" s="1"/>
+    <row r="182" spans="1:15">
+      <c r="O182" s="5"/>
+    </row>
+    <row r="190" spans="1:15">
+      <c r="L190" s="1"/>
+    </row>
+    <row r="195" spans="6:8" ht="15.75">
+      <c r="F195" s="3"/>
+      <c r="H195" s="3"/>
     </row>
     <row r="196" spans="6:8" ht="15.75">
       <c r="F196" s="3"/>
@@ -4866,14 +4853,10 @@
       <c r="F197" s="3"/>
       <c r="H197" s="3"/>
     </row>
-    <row r="198" spans="6:8" ht="15.75">
-      <c r="F198" s="3"/>
-      <c r="H198" s="3"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R198">
-    <sortCondition ref="A2:A198"/>
-    <sortCondition ref="B2:B198"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R197">
+    <sortCondition ref="A2:A197"/>
+    <sortCondition ref="B2:B197"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4882,10 +4865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138:L139"/>
+      <selection activeCell="A140" sqref="A140:M140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6340,6 +6323,23 @@
       </c>
       <c r="L139" s="1">
         <v>43661</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
+      <c r="A140" t="s">
+        <v>199</v>
+      </c>
+      <c r="B140">
+        <v>10</v>
+      </c>
+      <c r="D140" t="s">
+        <v>217</v>
+      </c>
+      <c r="G140" t="s">
+        <v>262</v>
+      </c>
+      <c r="L140" s="8">
+        <v>43986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>